<commit_message>
Change a single G4 -40° value
Changed to something other than zero (0.310792). This way students will be able to use wilcox_test on the pairwise comparisons without any problems popping up when doing the KW post-hoc. No more comparing 2 groups of all zero's.
</commit_message>
<xml_diff>
--- a/practicum6/2017_11_22_data_Eveline_statistiek_tellingen_STUDENTEN.xlsx
+++ b/practicum6/2017_11_22_data_Eveline_statistiek_tellingen_STUDENTEN.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ggbilcke\Dropbox\dropboxStats1819\class6_nonPar\case\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CompOmics Gwen\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7E4429C-E117-4F74-B296-13D924C97958}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25596" windowHeight="14676"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="stat data" sheetId="4" r:id="rId1"/>
@@ -65,7 +66,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -190,13 +191,13 @@
     </xf>
   </cellXfs>
   <cellStyles count="16">
-    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="13" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="15" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -204,8 +205,8 @@
     <cellStyle name="Hyperlink" xfId="10" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="12" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="14" builtinId="8" hidden="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="normálne 2" xfId="1"/>
+    <cellStyle name="normálne 2" xfId="1" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -242,7 +243,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -317,6 +318,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -352,6 +370,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -527,24 +562,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E121"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D110" sqref="D110"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.33203125" customWidth="1"/>
-    <col min="2" max="3" width="14.44140625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="17.28515625" customWidth="1"/>
+    <col min="2" max="3" width="14.42578125" style="2" customWidth="1"/>
     <col min="4" max="4" width="22" style="12" customWidth="1"/>
-    <col min="5" max="5" width="15.77734375" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.77734375" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>10</v>
       </c>
@@ -561,7 +596,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>9</v>
       </c>
@@ -578,7 +613,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>9</v>
       </c>
@@ -595,7 +630,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>9</v>
       </c>
@@ -612,7 +647,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>9</v>
       </c>
@@ -629,7 +664,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>9</v>
       </c>
@@ -646,7 +681,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>9</v>
       </c>
@@ -663,7 +698,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>9</v>
       </c>
@@ -680,7 +715,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>9</v>
       </c>
@@ -697,7 +732,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>9</v>
       </c>
@@ -714,7 +749,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>9</v>
       </c>
@@ -731,7 +766,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>9</v>
       </c>
@@ -748,7 +783,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>9</v>
       </c>
@@ -765,7 +800,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>9</v>
       </c>
@@ -782,7 +817,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>9</v>
       </c>
@@ -799,7 +834,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
         <v>9</v>
       </c>
@@ -816,7 +851,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>9</v>
       </c>
@@ -833,7 +868,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
         <v>9</v>
       </c>
@@ -850,7 +885,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
         <v>9</v>
       </c>
@@ -867,7 +902,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
         <v>9</v>
       </c>
@@ -884,7 +919,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
         <v>9</v>
       </c>
@@ -901,7 +936,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
         <v>9</v>
       </c>
@@ -918,7 +953,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
         <v>9</v>
       </c>
@@ -935,7 +970,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
         <v>9</v>
       </c>
@@ -952,7 +987,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
         <v>9</v>
       </c>
@@ -969,7 +1004,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
         <v>9</v>
       </c>
@@ -986,7 +1021,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
         <v>9</v>
       </c>
@@ -1003,7 +1038,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
         <v>9</v>
       </c>
@@ -1020,7 +1055,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
         <v>9</v>
       </c>
@@ -1037,7 +1072,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
         <v>9</v>
       </c>
@@ -1054,7 +1089,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
         <v>9</v>
       </c>
@@ -1071,7 +1106,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
         <v>9</v>
       </c>
@@ -1088,7 +1123,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
         <v>9</v>
       </c>
@@ -1105,7 +1140,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
         <v>9</v>
       </c>
@@ -1122,7 +1157,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
         <v>9</v>
       </c>
@@ -1139,7 +1174,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
         <v>9</v>
       </c>
@@ -1156,7 +1191,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="8" t="s">
         <v>9</v>
       </c>
@@ -1173,7 +1208,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="8" t="s">
         <v>9</v>
       </c>
@@ -1190,7 +1225,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="8" t="s">
         <v>9</v>
       </c>
@@ -1207,7 +1242,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="8" t="s">
         <v>9</v>
       </c>
@@ -1224,7 +1259,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="8" t="s">
         <v>9</v>
       </c>
@@ -1241,7 +1276,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="8" t="s">
         <v>9</v>
       </c>
@@ -1258,7 +1293,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="8" t="s">
         <v>9</v>
       </c>
@@ -1275,7 +1310,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="8" t="s">
         <v>9</v>
       </c>
@@ -1292,7 +1327,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="8" t="s">
         <v>9</v>
       </c>
@@ -1309,7 +1344,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="8" t="s">
         <v>9</v>
       </c>
@@ -1326,7 +1361,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="8" t="s">
         <v>9</v>
       </c>
@@ -1343,7 +1378,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="8" t="s">
         <v>9</v>
       </c>
@@ -1360,7 +1395,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="8" t="s">
         <v>9</v>
       </c>
@@ -1377,7 +1412,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="8" t="s">
         <v>9</v>
       </c>
@@ -1394,7 +1429,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="8" t="s">
         <v>9</v>
       </c>
@@ -1411,7 +1446,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="8" t="s">
         <v>9</v>
       </c>
@@ -1428,7 +1463,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="8" t="s">
         <v>9</v>
       </c>
@@ -1445,7 +1480,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="8" t="s">
         <v>9</v>
       </c>
@@ -1462,7 +1497,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="8" t="s">
         <v>9</v>
       </c>
@@ -1479,7 +1514,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="8" t="s">
         <v>9</v>
       </c>
@@ -1496,7 +1531,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="8" t="s">
         <v>9</v>
       </c>
@@ -1513,7 +1548,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="8" t="s">
         <v>9</v>
       </c>
@@ -1530,7 +1565,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="8" t="s">
         <v>9</v>
       </c>
@@ -1547,7 +1582,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="8" t="s">
         <v>9</v>
       </c>
@@ -1564,7 +1599,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="8" t="s">
         <v>9</v>
       </c>
@@ -1581,7 +1616,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="8" t="s">
         <v>9</v>
       </c>
@@ -1598,7 +1633,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="8" t="s">
         <v>9</v>
       </c>
@@ -1615,7 +1650,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="8" t="s">
         <v>9</v>
       </c>
@@ -1632,7 +1667,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="8" t="s">
         <v>9</v>
       </c>
@@ -1649,7 +1684,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="8" t="s">
         <v>9</v>
       </c>
@@ -1666,7 +1701,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="8" t="s">
         <v>9</v>
       </c>
@@ -1683,7 +1718,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="8" t="s">
         <v>9</v>
       </c>
@@ -1700,7 +1735,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="8" t="s">
         <v>9</v>
       </c>
@@ -1717,7 +1752,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="8" t="s">
         <v>9</v>
       </c>
@@ -1734,7 +1769,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="8" t="s">
         <v>9</v>
       </c>
@@ -1751,7 +1786,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="8" t="s">
         <v>9</v>
       </c>
@@ -1768,7 +1803,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="8" t="s">
         <v>9</v>
       </c>
@@ -1785,7 +1820,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="8" t="s">
         <v>9</v>
       </c>
@@ -1802,7 +1837,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="8" t="s">
         <v>9</v>
       </c>
@@ -1819,7 +1854,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="8" t="s">
         <v>9</v>
       </c>
@@ -1836,7 +1871,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="8" t="s">
         <v>9</v>
       </c>
@@ -1853,7 +1888,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="8" t="s">
         <v>9</v>
       </c>
@@ -1870,7 +1905,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="8" t="s">
         <v>9</v>
       </c>
@@ -1887,7 +1922,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="8" t="s">
         <v>9</v>
       </c>
@@ -1904,7 +1939,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="8" t="s">
         <v>9</v>
       </c>
@@ -1921,7 +1956,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="8" t="s">
         <v>9</v>
       </c>
@@ -1938,7 +1973,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="8" t="s">
         <v>9</v>
       </c>
@@ -1955,7 +1990,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="8" t="s">
         <v>9</v>
       </c>
@@ -1972,7 +2007,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="8" t="s">
         <v>9</v>
       </c>
@@ -1989,7 +2024,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="8" t="s">
         <v>9</v>
       </c>
@@ -2006,7 +2041,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="8" t="s">
         <v>9</v>
       </c>
@@ -2023,7 +2058,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="8" t="s">
         <v>9</v>
       </c>
@@ -2040,7 +2075,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="8" t="s">
         <v>9</v>
       </c>
@@ -2057,7 +2092,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="8" t="s">
         <v>9</v>
       </c>
@@ -2074,7 +2109,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="8" t="s">
         <v>9</v>
       </c>
@@ -2091,7 +2126,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="8" t="s">
         <v>9</v>
       </c>
@@ -2108,7 +2143,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="8" t="s">
         <v>9</v>
       </c>
@@ -2125,7 +2160,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="8" t="s">
         <v>9</v>
       </c>
@@ -2142,7 +2177,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="8" t="s">
         <v>9</v>
       </c>
@@ -2159,7 +2194,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="8" t="s">
         <v>9</v>
       </c>
@@ -2176,7 +2211,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="8" t="s">
         <v>9</v>
       </c>
@@ -2193,7 +2228,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="8" t="s">
         <v>0</v>
       </c>
@@ -2210,7 +2245,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="8" t="s">
         <v>0</v>
       </c>
@@ -2227,7 +2262,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="8" t="s">
         <v>0</v>
       </c>
@@ -2244,7 +2279,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="8" t="s">
         <v>0</v>
       </c>
@@ -2261,7 +2296,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="8" t="s">
         <v>0</v>
       </c>
@@ -2278,7 +2313,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="8" t="s">
         <v>0</v>
       </c>
@@ -2295,7 +2330,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="8" t="s">
         <v>0</v>
       </c>
@@ -2312,7 +2347,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="8" t="s">
         <v>0</v>
       </c>
@@ -2329,7 +2364,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="8" t="s">
         <v>0</v>
       </c>
@@ -2346,7 +2381,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="8" t="s">
         <v>0</v>
       </c>
@@ -2363,7 +2398,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="8" t="s">
         <v>0</v>
       </c>
@@ -2380,7 +2415,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="8" t="s">
         <v>0</v>
       </c>
@@ -2397,7 +2432,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="8" t="s">
         <v>0</v>
       </c>
@@ -2408,13 +2443,13 @@
         <v>2</v>
       </c>
       <c r="D110" s="12">
-        <v>0</v>
+        <v>0.31079200000000001</v>
       </c>
       <c r="E110" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="8" t="s">
         <v>0</v>
       </c>
@@ -2431,7 +2466,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="8" t="s">
         <v>0</v>
       </c>
@@ -2448,7 +2483,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="8" t="s">
         <v>0</v>
       </c>
@@ -2465,7 +2500,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" s="8" t="s">
         <v>0</v>
       </c>
@@ -2482,7 +2517,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="8" t="s">
         <v>0</v>
       </c>
@@ -2499,7 +2534,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="8" t="s">
         <v>0</v>
       </c>
@@ -2516,7 +2551,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" s="8" t="s">
         <v>0</v>
       </c>
@@ -2533,7 +2568,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" s="8" t="s">
         <v>0</v>
       </c>
@@ -2550,7 +2585,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" s="8" t="s">
         <v>0</v>
       </c>
@@ -2567,7 +2602,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" s="8" t="s">
         <v>0</v>
       </c>
@@ -2584,7 +2619,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="8" t="s">
         <v>0</v>
       </c>
@@ -2602,8 +2637,8 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E25"/>
-  <sortState ref="A2:I553">
+  <autoFilter ref="A1:E25" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I553">
     <sortCondition ref="A2:A553"/>
     <sortCondition descending="1" ref="C2:C553"/>
   </sortState>

</xml_diff>